<commit_message>
Add contract case to createDoc util function
</commit_message>
<xml_diff>
--- a/files/input/companiesData.xlsx
+++ b/files/input/companiesData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>companyNip</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>PALOMINO Justyna Jaskulska</t>
+  </si>
+  <si>
+    <t>isLegalPerson</t>
+  </si>
+  <si>
+    <t>isNaturalPerson</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -355,22 +364,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,39 +388,54 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5252516964</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7720100638</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8982126450</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
         <v>5</v>
       </c>
     </row>

</xml_diff>